<commit_message>
pom file update & password removed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestEmailList.xlsx
+++ b/src/test/resources/TestEmailList.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Email\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19752" windowHeight="4992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,52 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>komal.pal@affle.com</t>
-  </si>
-  <si>
-    <t>achandel@charterglobal.com</t>
-  </si>
-  <si>
-    <t>careers@focussoftnet.com</t>
-  </si>
-  <si>
-    <t>minakshi@rsplacements.com</t>
-  </si>
-  <si>
-    <t>recruit@innovacx.com</t>
-  </si>
-  <si>
-    <t>skavya@hiringhut.in</t>
-  </si>
-  <si>
-    <t>sneha.m@wsneconsulting.com</t>
-  </si>
-  <si>
-    <t>sumaiya.sultana@adecco.com</t>
-  </si>
-  <si>
-    <t>amulya.bijur@tailwebs.com</t>
-  </si>
-  <si>
-    <t>florence.g@fluentgrid.com</t>
-  </si>
-  <si>
-    <t>hr1amrutha@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indira.somala@resolver.com </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,14 +41,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,53 +69,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -470,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,106 +402,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sortState ref="A3:A23">
-    <sortCondition ref="A2"/>
-  </sortState>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A8">
-    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A14">
-    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A14" r:id="rId4"/>
-    <hyperlink ref="A12" r:id="rId5"/>
-    <hyperlink ref="A3" r:id="rId6"/>
-    <hyperlink ref="A10" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A11" r:id="rId9"/>
-    <hyperlink ref="A7" r:id="rId10"/>
-    <hyperlink ref="A4" r:id="rId11"/>
-    <hyperlink ref="A6" r:id="rId12"/>
-    <hyperlink ref="A8" r:id="rId13"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>